<commit_message>
Fix: Faculty Page data leakage, Double Dr bug, and Modal synchronization. Corrected yearwise routing for MBA, MCA, CIVIL, and EVT.
</commit_message>
<xml_diff>
--- a/public/2025-26 Faculty Directory/ce, mba & mca sTAFF lIST updated.xlsx
+++ b/public/2025-26 Faculty Directory/ce, mba & mca sTAFF lIST updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSE_DEAN\Desktop\nriit-generativeai-campus\public\2025-26 Faculty Directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23E5F275-98B8-4B9E-8862-FA7559FFA266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8BF988-26C5-40F8-BF91-F41A5CDA3673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCFB3FE1-AB32-4D23-A341-9CB434C4A104}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CCFB3FE1-AB32-4D23-A341-9CB434C4A104}"/>
   </bookViews>
   <sheets>
     <sheet name="CE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="145">
   <si>
     <t>Dr.K.SRINIVASU</t>
   </si>
@@ -359,15 +359,9 @@
     <t>Fin/IT</t>
   </si>
   <si>
-    <t>Dr.RAVIKINDI SAI SANDEEP KUMAR</t>
-  </si>
-  <si>
     <t>MBA., Ph.D</t>
   </si>
   <si>
-    <t>12.08.2024</t>
-  </si>
-  <si>
     <t>DFAPS7024N</t>
   </si>
   <si>
@@ -471,6 +465,12 @@
   </si>
   <si>
     <t>ABRPO9060E</t>
+  </si>
+  <si>
+    <t>Dr KPR Rajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7-7-2025.</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5517B0C-D0D7-4EC5-BC97-14BACD2C3041}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,17 +1806,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1824,15 +1824,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F05896-9F44-4188-977F-68464A7B6199}">
-  <dimension ref="B2:M18"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1964,7 +1965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="48" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>3</v>
       </c>
@@ -1978,25 +1979,25 @@
         <v>106</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>99</v>
       </c>
       <c r="K6" s="3">
-        <v>976103652114</v>
+        <v>976503655114</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M6" s="3">
         <v>18</v>
@@ -2016,7 +2017,7 @@
         <v>95</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>97</v>
@@ -2025,7 +2026,7 @@
         <v>98</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>99</v>
@@ -2034,13 +2035,13 @@
         <v>713503973119</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M7" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="48" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>5</v>
       </c>
@@ -2051,34 +2052,34 @@
         <v>94</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="K8" s="3">
-        <v>270068204106</v>
+        <v>713503973119</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="M8" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>6</v>
       </c>
@@ -2089,34 +2090,34 @@
         <v>94</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K9" s="3">
-        <v>486189260489</v>
+        <v>270068204106</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M9" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>7</v>
       </c>
@@ -2127,34 +2128,34 @@
         <v>94</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K10" s="3">
-        <v>428393891089</v>
+        <v>486189260489</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="M10" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>8</v>
       </c>
@@ -2165,10 +2166,10 @@
         <v>94</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>103</v>
@@ -2176,20 +2177,20 @@
       <c r="H11" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I11" s="4">
-        <v>44447</v>
+      <c r="I11" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="3">
-        <v>373735246878</v>
+        <v>428393891089</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M11" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="24" x14ac:dyDescent="0.25">
@@ -2203,10 +2204,10 @@
         <v>94</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>103</v>
@@ -2215,19 +2216,19 @@
         <v>94</v>
       </c>
       <c r="I12" s="4">
-        <v>42741</v>
+        <v>44447</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K12" s="3">
-        <v>849206308234</v>
+        <v>373735246878</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="M12" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="24" x14ac:dyDescent="0.25">
@@ -2241,10 +2242,10 @@
         <v>94</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>103</v>
@@ -2253,16 +2254,16 @@
         <v>94</v>
       </c>
       <c r="I13" s="4">
-        <v>45430</v>
+        <v>42741</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="3">
-        <v>365313765898</v>
+        <v>849206308234</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="M13" s="3">
         <v>7</v>
@@ -2279,31 +2280,31 @@
         <v>94</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>134</v>
+        <v>94</v>
+      </c>
+      <c r="I14" s="4">
+        <v>45430</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="K14" s="3">
-        <v>226217518170</v>
+        <v>365313765898</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M14" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="24" x14ac:dyDescent="0.25">
@@ -2317,34 +2318,34 @@
         <v>94</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>136</v>
+        <v>112</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>103</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="4">
-        <v>44447</v>
+        <v>107</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="K15" s="3">
-        <v>339320558339</v>
+        <v>226217518170</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M15" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>13</v>
       </c>
@@ -2355,10 +2356,10 @@
         <v>94</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>103</v>
@@ -2367,22 +2368,22 @@
         <v>94</v>
       </c>
       <c r="I16" s="4">
-        <v>45297</v>
+        <v>44447</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K16" s="3">
-        <v>602135466543</v>
+        <v>339320558339</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="M16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>14</v>
       </c>
@@ -2393,10 +2394,10 @@
         <v>94</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>103</v>
@@ -2405,22 +2406,22 @@
         <v>94</v>
       </c>
       <c r="I17" s="4">
-        <v>44929</v>
+        <v>45297</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>35</v>
       </c>
       <c r="K17" s="3">
-        <v>599410820715</v>
+        <v>602135466543</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M17" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="36" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="24" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>15</v>
       </c>
@@ -2431,10 +2432,10 @@
         <v>94</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>103</v>
@@ -2443,34 +2444,72 @@
         <v>94</v>
       </c>
       <c r="I18" s="4">
+        <v>44929</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="3">
+        <v>599410820715</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M18" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="24" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="4">
         <v>42772</v>
       </c>
-      <c r="J18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="3">
+      <c r="J19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="3">
         <v>200700086105</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="M18" s="3">
+      <c r="L19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="M19" s="3">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>